<commit_message>
STM32: Added temp. regulation and prepared support for scroll buffers, minor restructuring
</commit_message>
<xml_diff>
--- a/STM32/FIAControl/UART Protocol.xlsx
+++ b/STM32/FIAControl/UART Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Dokumente\Elektronik\Projekte\funkwerk KJ LCD FIA\STM32\FIAControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E6EC0B-FC90-455F-9D52-1C22929DE3F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A63CCE-BAA3-4812-B9A3-8B6198F55616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4380" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>Frame Structure</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t>Sensors</t>
-  </si>
-  <si>
-    <t>LCD</t>
   </si>
   <si>
     <t>0x42</t>
@@ -309,6 +306,55 @@
 Byte 1 - Side A contrast low byte
 Byte 2 - Side B contrast high byte
 Byte 3 - Side B contrast low byte</t>
+  </si>
+  <si>
+    <t>LCDs</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>CREATE_SCROLL_BUFFER</t>
+  </si>
+  <si>
+    <t>Create a scroll buffer.
+Parameters:
+Byte 0 - X position high byte
+Byte 1 - X position low byte
+Byte 2 - Y position high byte
+Byte 3 - Y position low byte
+Byte 4 - Width high byte
+Byte 5 - Width low byte
+Byte 6 - Height high byte
+Byte 7 - Height low byte
+Response:
+Byte 0 - The ID of the created buffer or 0 on failure</t>
+  </si>
+  <si>
+    <t>0x61</t>
+  </si>
+  <si>
+    <t>DELETE_SCROLL_BUFFER</t>
+  </si>
+  <si>
+    <t>Delete a scroll buffer.
+Parameters:
+Byte 0 - The ID of the buffer to be deleted
+Response:
+Byte 0 - 1 on success, 0 on failure</t>
+  </si>
+  <si>
+    <t>0x62</t>
+  </si>
+  <si>
+    <t>SET_DESTINATION_BUFFER</t>
+  </si>
+  <si>
+    <t>Set the SPI destination buffer.
+Parameters:
+Byte 0 - The ID of the destination buffer
+Response:
+Byte 0 - 1 on success, 0 on failure</t>
   </si>
 </sst>
 </file>
@@ -726,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +807,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
@@ -784,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -802,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -856,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -890,7 +936,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -910,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -944,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -978,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1012,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1048,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="150" x14ac:dyDescent="0.25">
@@ -1068,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -1086,13 +1132,13 @@
         <v>2</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -1104,12 +1150,12 @@
         <v>4</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>33</v>
@@ -1124,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -1143,14 +1189,56 @@
       </c>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="3"/>
+    <row r="26" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>

</xml_diff>

<commit_message>
STM32: Actual scroll implementation, update protocol doc
</commit_message>
<xml_diff>
--- a/STM32/FIAControl/UART Protocol.xlsx
+++ b/STM32/FIAControl/UART Protocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Dokumente\Elektronik\Projekte\funkwerk KJ LCD FIA\STM32\FIAControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A63CCE-BAA3-4812-B9A3-8B6198F55616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E0965D-F39E-4117-965C-BAC88B0BCCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4380" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,23 @@
     <sheet name="General Information" sheetId="2" r:id="rId1"/>
     <sheet name="UART Commands" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>Frame Structure</t>
   </si>
@@ -317,20 +323,6 @@
     <t>CREATE_SCROLL_BUFFER</t>
   </si>
   <si>
-    <t>Create a scroll buffer.
-Parameters:
-Byte 0 - X position high byte
-Byte 1 - X position low byte
-Byte 2 - Y position high byte
-Byte 3 - Y position low byte
-Byte 4 - Width high byte
-Byte 5 - Width low byte
-Byte 6 - Height high byte
-Byte 7 - Height low byte
-Response:
-Byte 0 - The ID of the created buffer or 0 on failure</t>
-  </si>
-  <si>
     <t>0x61</t>
   </si>
   <si>
@@ -353,6 +345,72 @@
     <t>Set the SPI destination buffer.
 Parameters:
 Byte 0 - The ID of the destination buffer
+Response:
+Byte 0 - 1 on success, 0 on failure</t>
+  </si>
+  <si>
+    <t>0x63</t>
+  </si>
+  <si>
+    <t>UPDATE_SCROLL_BUFFER</t>
+  </si>
+  <si>
+    <t>Create a scroll buffer. Position and size values are in pixels. X and Y are counted from the top-left corner of the display.
+Parameters:
+Byte 0 - Display X position high byte
+Byte 1 - Display side
+Byte 2 - Display X position low byte
+Byte 3 - Display Y position high byte
+Byte 4 - Dispaly Y position low byte
+Byte 5 - Display width high byte
+Byte 6 - Display width low byte
+Byte 7 - Display height high byte
+Byte 8 - Display height low byte
+Byte 9 - Internal width high byte
+Byte 10 - Internal width low byte
+Byte 11 - Internal height high byte
+Byte 12 - Internal height low byte
+Byte 13 - Scroll offset X high byte
+Byte 14 - Scroll offset X low byte
+Byte 15 - Scroll offset Y high byte
+Byte 16 - Scroll offset Y low byte
+Byte 17 - Scroll speed X high byte
+Byte 18 - Scroll speed X low byte
+Byte 19 - Scroll speed Y high byte
+Byte 20 - Scroll speed Y low byte
+Byte 21 - Scroll step X high byte
+Byte 22 - Scroll step X low byte
+Byte 23 - Scroll step Y high byte
+Byte 24 - Scroll step Y low byte
+Response:
+Byte 0 - The ID of the created buffer or 0 on failure</t>
+  </si>
+  <si>
+    <t>Update parameters of a scroll buffer. Position and size values are in pixels. X and Y are counted from the top-left corner of the display.
+Set any value to 0xFFFF (0x7FFF for scroll steps) to leave unchanged.
+Parameters:
+Byte 0 - The ID of the buffer to be updated
+Byte 1 - Display side
+Byte 2 - Display X position high byte
+Byte 3 - Display X position low byte
+Byte 4 - Display Y position high byte
+Byte 5 - Dispaly Y position low byte
+Byte 6 - Display width high byte
+Byte 7 - Display width low byte
+Byte 8 - Display height high byte
+Byte 9 - Display height low byte
+Byte 10 - Scroll offset X high byte
+Byte 11 - Scroll offset X low byte
+Byte 12 - Scroll offset Y high byte
+Byte 13 - Scroll offset Y low byte
+Byte 14 - Scroll speed X high byte
+Byte 15 - Scroll speed X low byte
+Byte 16 - Scroll speed Y high byte
+Byte 17 - Scroll speed Y low byte
+Byte 18 - Scroll step X high byte
+Byte 19 - Scroll step X low byte
+Byte 20 - Scroll step Y high byte
+Byte 21 - Scroll step Y low byte
 Response:
 Byte 0 - 1 on success, 0 on failure</t>
   </si>
@@ -412,13 +470,13 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,18 +830,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="98.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="130.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -814,7 +872,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -829,12 +887,12 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
@@ -847,12 +905,12 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -867,12 +925,12 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -885,10 +943,10 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="2:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
@@ -901,12 +959,12 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
@@ -919,10 +977,10 @@
       <c r="F10">
         <v>4</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
@@ -935,12 +993,12 @@
       <c r="F11">
         <v>4</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -955,12 +1013,12 @@
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
@@ -973,10 +1031,10 @@
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
@@ -989,12 +1047,12 @@
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1007,10 +1065,10 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" s="8"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1023,12 +1081,12 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1041,10 +1099,10 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17" s="8"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
@@ -1057,12 +1115,12 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
@@ -1075,10 +1133,10 @@
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1093,12 +1151,12 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1113,12 +1171,12 @@
       <c r="F21">
         <v>8</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
@@ -1131,12 +1189,12 @@
       <c r="F22">
         <v>2</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="3" t="s">
         <v>62</v>
       </c>
@@ -1149,12 +1207,12 @@
       <c r="F23">
         <v>4</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1169,12 +1227,12 @@
       <c r="F24">
         <v>0</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3" t="s">
         <v>34</v>
       </c>
@@ -1187,9 +1245,9 @@
       <c r="F25">
         <v>4</v>
       </c>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="2:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>79</v>
       </c>
@@ -1197,51 +1255,65 @@
         <v>80</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>81</v>
+      <c r="G26" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" t="s">
         <v>82</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" t="s">
         <v>85</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="7" t="s">
+    </row>
+    <row r="29" spans="2:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29">
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
STM32: Make mask optional, reorder cmds, add GET_DESTINATION_BUFFER cmd
</commit_message>
<xml_diff>
--- a/STM32/FIAControl/UART Protocol.xlsx
+++ b/STM32/FIAControl/UART Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Dokumente\Elektronik\Projekte\funkwerk KJ LCD FIA\STM32\FIAControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E0965D-F39E-4117-965C-BAC88B0BCCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B7F9D0-F446-41DD-AEA9-1CF25C85D35D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4380" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>Frame Structure</t>
   </si>
@@ -413,6 +413,39 @@
 Byte 21 - Scroll step Y low byte
 Response:
 Byte 0 - 1 on success, 0 on failure</t>
+  </si>
+  <si>
+    <t>0x64</t>
+  </si>
+  <si>
+    <t>GET_DESTINATION_BUFFER</t>
+  </si>
+  <si>
+    <t>Get the SPI destination buffer.
+Response:
+Byte 0 - The buffer ID as expected by SET_DESTINATION_BUFFER</t>
+  </si>
+  <si>
+    <t>SET_MASK_ENABLED</t>
+  </si>
+  <si>
+    <t>GET_MASK_ENABLED</t>
+  </si>
+  <si>
+    <t>0x65</t>
+  </si>
+  <si>
+    <t>0x66</t>
+  </si>
+  <si>
+    <t>Set mask compositing on or off.
+Parameters:
+Byte 0 - 1 for on, 0 for off</t>
+  </si>
+  <si>
+    <t>Return mask compositing state.
+Response:
+Byte 0 - 1 for on, 0 for off</t>
   </si>
 </sst>
 </file>
@@ -828,10 +861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G29"/>
+  <dimension ref="B2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,38 +1314,89 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="405" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="405" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E29">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>